<commit_message>
Updated Input files and Indexes
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0B73E6-28C4-F44C-A188-F90FD492063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E919F5AF-8ED2-574C-8859-25940B24BF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="-880" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -98,64 +98,6 @@
     df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
 WHERE 
     st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever';</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    sf.file_name AS "File Name",
-    sf.file_type AS "File Type",
-    'study' AS "Association",
-    sf.file_description AS "Description",
-    CASE
-        WHEN sf.file_name LIKE '%.bai' THEN 'bai'
-        WHEN sf.file_name LIKE '%.bam' THEN 'bam'
-        WHEN sf.file_name LIKE '%.csv' THEN 'csv'
-        WHEN sf.file_name LIKE '%.doc' THEN 'doc'
-        WHEN sf.file_name LIKE '%.docx' THEN 'docx'
-        WHEN sf.file_name LIKE '%.gz' THEN 'gz'
-        WHEN sf.file_name LIKE '%.pdf' THEN 'pdf'
-        WHEN sf.file_name LIKE '%.rtf' THEN 'rtf'
-        WHEN sf.file_name LIKE '%.tbi' THEN 'tbi'
-        WHEN sf.file_name LIKE '%.tif' THEN 'tif'
-        WHEN sf.file_name LIKE '%.xls' THEN 'xls'
-        WHEN sf.file_name LIKE '%.xlsx' THEN 'xlsx'
-        ELSE 'Unknown'
-    END AS "Format",
-    CASE     
-        WHEN sf.original_file_size &gt;= 1024 * 1024 * 1024 THEN 
-            ROUND(sf.original_file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-        WHEN sf.original_file_size &gt;= 1024 * 1024 THEN 
-            ROUND(sf.original_file_size / (1024.0 * 1024.0), 2) || ' MB' 
-        WHEN sf.original_file_size &gt;= 1024 THEN 
-            ROUND(sf.original_file_size / 1024.0, 2) || ' KB' 
-        ELSE 
-            ROUND(sf.original_file_size, 2) || ' Bytes' 
-    END AS "Size",
-    st.clinical_study_designation AS "Study Code"
-FROM 
-    df_case_file cf
-JOIN 
-    df_sample smp ON cf."sample.sample_id" = smp.sample_id
-JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
-ORDER BY 
-    sf.file_name ASC
-LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -279,6 +221,64 @@
     c.case_id AS "Case ID",
     dmg.breed AS "Breed",
     diag.disease_term AS "Diagnosis"
+FROM 
+    df_case_file cf
+JOIN 
+    df_sample smp ON cf."sample.sample_id" = smp.sample_id
+JOIN 
+    df_case c ON smp."case.case_id" = c.case_id
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_demographic dmg ON dmg."case.case_id" = c.case_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_id" = c.case_id
+JOIN 
+    df_enrollment enr ON enr."case.case_id" = c.case_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
+ORDER BY 
+    sf.file_name ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    sf.file_name AS "File Name",
+    sf.file_type AS "File Type",
+    'study' AS "Association",
+    sf.file_description AS "Description",
+    CASE
+        WHEN sf.file_name LIKE '%.bai' THEN 'bai'
+        WHEN sf.file_name LIKE '%.bam' THEN 'bam'
+        WHEN sf.file_name LIKE '%.csv' THEN 'csv'
+        WHEN sf.file_name LIKE '%.doc' THEN 'doc'
+        WHEN sf.file_name LIKE '%.docx' THEN 'docx'
+        WHEN sf.file_name LIKE '%.gz' THEN 'gz'
+        WHEN sf.file_name LIKE '%.pdf' THEN 'pdf'
+        WHEN sf.file_name LIKE '%.rtf' THEN 'rtf'
+        WHEN sf.file_name LIKE '%.tbi' THEN 'tbi'
+        WHEN sf.file_name LIKE '%.tif' THEN 'tif'
+        WHEN sf.file_name LIKE '%.xls' THEN 'xls'
+        WHEN sf.file_name LIKE '%.xlsx' THEN 'xlsx'
+        ELSE 'Unknown'
+    END AS "Format",
+    CASE     
+        WHEN sf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
+        WHEN sf.file_size &gt;= 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
+        WHEN sf.file_size &gt;= 1024 THEN 
+            ROUND(sf.file_size / 1024.0, 2) || ' KB' 
+        ELSE 
+            ROUND(sf.file_size, 2) || ' Bytes' 
+    END AS "Size",
+    st.clinical_study_designation AS "Study Code"
 FROM 
     df_case_file cf
 JOIN 
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -766,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -775,7 +775,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added CCDI framework scripts
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E919F5AF-8ED2-574C-8859-25940B24BF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476671E-8342-3D46-A2E6-1FFB0B252096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="-880" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>CaseFilesTab</t>
-  </si>
-  <si>
-    <t>TC01_ICDC_TLC01_Breed-GoldenRetriever_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_ICDC_TLC01_Breed-GoldenRetriever_WebData.xlsx</t>
   </si>
   <si>
     <t>SELECT
@@ -304,6 +298,12 @@
 ORDER BY 
     sf.file_name ASC
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_WebData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,16 +749,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -766,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -775,7 +775,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated ICDC properties and indexes
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_TCL01_Breed-GoldenRetriever.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476671E-8342-3D46-A2E6-1FFB0B252096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13062C25-70D8-CE4B-94B2-5B18F7232862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="-880" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-46560" yWindow="-4940" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,10 +65,16 @@
     <t>CaseFilesTab</t>
   </si>
   <si>
+    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_WebData.xlsx</t>
+  </si>
+  <si>
     <t>SELECT
     COUNT(DISTINCT p.program_acronym) AS "Programs",
     COUNT(DISTINCT st.clinical_study_designation) AS "Studies",
-    COUNT(DISTINCT c.case_id) AS "Cases",
+    COUNT(DISTINCT c.case_record_id) AS "Cases",
     COUNT(DISTINCT smp.sample_id) AS "Samples",
     COUNT(DISTINCT cf.file_name) AS "Case Files",         
     COUNT(DISTINCT sf.file_name) AS "Study Files" 
@@ -79,13 +85,13 @@
 JOIN 
     df_case c ON st.clinical_study_designation = c."study.clinical_study_designation"
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_sample smp ON smp."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
 LEFT JOIN 
     df_case_file cf ON cf."sample.sample_id" = smp.sample_id
 LEFT JOIN 
@@ -94,50 +100,10 @@
     st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever';</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    c.case_id AS "Case ID",
-    COALESCE(dmg.breed, '') AS "Breed",
-    COALESCE(diag.disease_term, '') AS "Diagnosis",
-    COALESCE(smp.sample_site, '') AS "Sample Site",
-    COALESCE(smp.summarized_sample_type, '') AS "Sample Type",
-    COALESCE(smp.specific_sample_pathology, '') AS "Pathology/Morphology",
-    COALESCE(smp.tumor_grade, '') AS "Tumor Grade",
-    COALESCE(smp.sample_chronology, '') AS "Sample Chronology",
-    COALESCE(smp.percentage_tumor, '') AS "Percentage Tumor",
-    COALESCE(smp.necropsy_sample, '') AS "Necropsy Sample",
-    COALESCE(smp.sample_preservation, '') AS "Sample Preservation"
-FROM 
-    df_sample smp
-JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE 
-   st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
-ORDER BY 
-    smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SELECT
-    DISTINCT c.case_id AS "Case ID",
-    st.clinical_study_designation AS "Study Code",
-    st.clinical_study_type AS "Study Type",
+    DISTINCT TRIM(c.case_record_id) AS "Case ID",
+    TRIM(st.clinical_study_designation) AS "Study Code",
+    TRIM(st.clinical_study_type) AS "Study Type",
     dmg.breed AS "Breed",
     diag.disease_term AS "Diagnosis",
     diag.stage_of_disease AS "Stage Of Disease",
@@ -157,15 +123,15 @@
 JOIN 
     df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
 JOIN 
     df_program p ON st."program.program_acronym" = p.program_acronym
 JOIN 
-    df_sample smp ON smp."case.case_id" = c.case_id
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 LEFT JOIN 
@@ -177,76 +143,15 @@
 WHERE
     st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
 ORDER BY 
-    c.case_id ASC
+    c.case_record_id ASC
 LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT DISTINCT
-    cf.file_name AS "File Name",
-    CASE
-        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
-        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
-        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
-        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
-        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
-        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
-        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
-        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
-        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
-        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
-        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
-        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
-        ELSE 'Unknown'
-    END AS "Format",
-    cf.file_type AS "File Type",
-    CASE     
-    WHEN cf.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-    WHEN cf.file_size &gt;= 1024 * 1024 THEN 
-        ROUND(cf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
-    WHEN cf.file_size &gt;= 1024 THEN 
-        ROUND(cf.file_size / 1024.0, 2) || ' KB' 
-    ELSE 
-        ROUND(cf.file_size, 2) || ' Bytes' 
-END AS "Size",
-    'sample' AS "Association",
-    cf.file_description AS "Description",
-    smp.sample_id AS "Sample ID",
-    c.case_id AS "Case ID",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis"
-FROM 
-    df_case_file cf
-JOIN 
-    df_sample smp ON cf."sample.sample_id" = smp.sample_id
-JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
-ORDER BY 
-    sf.file_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    sf.file_name AS "File Name",
-    sf.file_type AS "File Type",
+    TRIM(sf.file_name) AS "File Name",
+    TRIM(sf.file_type) AS "File Type",
     'study' AS "Association",
-    sf.file_description AS "Description",
+    TRIM(sf.file_description) AS "Description",
     CASE
         WHEN sf.file_name LIKE '%.bai' THEN 'bai'
         WHEN sf.file_name LIKE '%.bam' THEN 'bam'
@@ -278,17 +183,17 @@
 JOIN 
     df_sample smp ON cf."sample.sample_id" = smp.sample_id
 JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
+    df_case c ON smp."case.case_record_id" = c.case_record_id
 JOIN 
     df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
 JOIN 
     df_program p ON st."program.program_acronym" = p.program_acronym
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 LEFT JOIN 
@@ -300,10 +205,121 @@
 LIMIT 100;</t>
   </si>
   <si>
-    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_ICDC_TCL01_Breed-GoldenRetriever_WebData.xlsx</t>
+    <t>SELECT DISTINCT
+    smp.sample_id AS "Sample ID",
+    c.case_record_id AS "Case ID",
+    COALESCE(dmg.breed, '') AS "Breed",
+    COALESCE(diag.disease_term, '') AS "Diagnosis",
+    COALESCE(smp.sample_site, '') AS "Sample Site",
+    COALESCE(smp.summarized_sample_type, '') AS "Sample Type",
+    COALESCE(smp.specific_sample_pathology, '') AS "Pathology/Morphology",
+    COALESCE(smp.tumor_grade, '') AS "Tumor Grade",
+    COALESCE(smp.sample_chronology, '') AS "Sample Chronology",
+    COALESCE(smp.percentage_tumor, '') AS "Percentage Tumor",
+    COALESCE(TRIM(smp.necropsy_sample), '') AS "Necropsy Sample",
+    COALESCE(smp.sample_preservation, '') AS "Sample Preservation"
+FROM 
+    df_sample smp
+JOIN 
+    df_case c ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE 
+   st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
+ORDER BY 
+    smp.sample_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT 
+    DISTINCT cf.file_name AS "File Name",
+    CASE
+        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
+        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
+        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
+        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
+        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
+        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
+        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
+        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
+        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
+        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
+        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
+        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
+        ELSE 'Unknown'
+    END AS "Format",
+    cf.file_type AS "File Type",
+    CASE     
+    WHEN cf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+            ELSE ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+        END
+    WHEN cf.file_size &gt;= 1024 * 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(cf.file_size / (1024.0 * 1024.0), 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+            ELSE ROUND(cf.file_size / (1024.0 * 1024.0), 2) || ' MB'
+        END
+    WHEN cf.file_size &gt;= 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / 1024.0, 2) = CAST(ROUND(cf.file_size / 1024.0, 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+            ELSE ROUND(cf.file_size / 1024.0, 2) || ' KB'
+        END
+    ELSE 
+        CASE 
+            WHEN ROUND(cf.file_size, 2) = CAST(ROUND(cf.file_size, 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size, 0) AS INT) AS TEXT) || ' Bytes'
+            ELSE ROUND(cf.file_size, 2) || ' Bytes'
+        END
+END AS "Size",
+    'sample' AS "Association",
+    cf.file_description AS "Description",
+    smp.sample_id AS "Sample ID",
+    c.case_record_id AS "Case ID",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis"
+FROM 
+    df_case_file cf
+JOIN 
+    df_sample smp ON cf."sample.sample_id" = smp.sample_id
+JOIN 
+    df_case c ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'TCL01' AND dmg.breed = 'Golden Retriever'
+ORDER BY 
+    cf.file_name ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -715,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -748,25 +764,25 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -775,7 +791,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>

</xml_diff>